<commit_message>
Can deal now with double regions
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11FA2B4-FA8F-455E-8B10-43138E7F04C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D454C82-713E-45E5-B3B6-3641C155743D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -789,9 +789,6 @@
     <t>ModalType selected</t>
   </si>
   <si>
-    <t>Sectors</t>
-  </si>
-  <si>
     <t>Industry</t>
   </si>
   <si>
@@ -816,13 +813,16 @@
     <t>Sectors selected</t>
   </si>
   <si>
-    <t>Modal_type</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>ModalType</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1199,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
@@ -3154,13 +3154,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C358E473-EC7A-41C0-8602-044D340269A5}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>249</v>
@@ -3320,17 +3322,17 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3343,7 +3345,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3351,7 +3353,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3359,7 +3361,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3367,7 +3369,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3375,7 +3377,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3383,7 +3385,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3391,7 +3393,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3406,7 +3408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3414,7 +3416,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Fixed a lot of errors in the excel sheets: - duplicate data entries - empty rows Pivoting works but not yet for regions
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D454C82-713E-45E5-B3B6-3641C155743D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{073028ED-85D4-4E35-8EB7-3223E316B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="263">
   <si>
     <t>DE</t>
   </si>
@@ -823,6 +823,9 @@
   </si>
   <si>
     <t>ModalType</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -866,12 +869,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1186,18 +1190,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>258</v>
       </c>
@@ -1206,315 +1210,324 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
       <c r="B16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>31</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>33</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>34</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>37</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>1</v>
       </c>
     </row>
@@ -1531,12 +1544,12 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>185</v>
       </c>
@@ -1544,7 +1557,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1552,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1560,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1568,7 +1581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1576,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1584,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1592,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1600,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1608,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1616,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1624,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1632,7 +1645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1640,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1648,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1656,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1664,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1672,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -1680,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1688,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1696,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1712,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1720,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1728,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1736,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -1744,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -1752,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
@@ -1760,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>66</v>
       </c>
@@ -1768,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>67</v>
       </c>
@@ -1776,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
@@ -1784,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
@@ -1792,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
@@ -1800,7 +1813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>71</v>
       </c>
@@ -1808,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>72</v>
       </c>
@@ -1816,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>73</v>
       </c>
@@ -1824,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>74</v>
       </c>
@@ -1832,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -1840,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1848,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1856,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1864,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -1872,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>80</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -1888,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1896,7 +1909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>83</v>
       </c>
@@ -1904,7 +1917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -1912,7 +1925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -1920,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -1928,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -1936,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -1944,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -1952,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -1960,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -1968,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>92</v>
       </c>
@@ -1976,7 +1989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -1984,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -1992,7 +2005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -2000,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>97</v>
       </c>
@@ -2016,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>98</v>
       </c>
@@ -2024,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>99</v>
       </c>
@@ -2032,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>100</v>
       </c>
@@ -2040,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -2048,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>102</v>
       </c>
@@ -2056,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>103</v>
       </c>
@@ -2064,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>104</v>
       </c>
@@ -2072,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>105</v>
       </c>
@@ -2080,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>106</v>
       </c>
@@ -2088,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -2096,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>108</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>109</v>
       </c>
@@ -2112,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>110</v>
       </c>
@@ -2120,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>111</v>
       </c>
@@ -2128,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>112</v>
       </c>
@@ -2136,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>113</v>
       </c>
@@ -2144,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>114</v>
       </c>
@@ -2152,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>115</v>
       </c>
@@ -2160,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>116</v>
       </c>
@@ -2168,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>117</v>
       </c>
@@ -2176,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>118</v>
       </c>
@@ -2184,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>119</v>
       </c>
@@ -2192,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>120</v>
       </c>
@@ -2200,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>121</v>
       </c>
@@ -2208,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>122</v>
       </c>
@@ -2216,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>123</v>
       </c>
@@ -2224,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>124</v>
       </c>
@@ -2232,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>125</v>
       </c>
@@ -2240,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>126</v>
       </c>
@@ -2248,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>127</v>
       </c>
@@ -2256,7 +2269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>128</v>
       </c>
@@ -2264,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>129</v>
       </c>
@@ -2272,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>130</v>
       </c>
@@ -2280,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>131</v>
       </c>
@@ -2288,7 +2301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>132</v>
       </c>
@@ -2296,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>133</v>
       </c>
@@ -2304,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>134</v>
       </c>
@@ -2312,7 +2325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>135</v>
       </c>
@@ -2320,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>136</v>
       </c>
@@ -2328,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>137</v>
       </c>
@@ -2336,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>138</v>
       </c>
@@ -2344,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>139</v>
       </c>
@@ -2352,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>140</v>
       </c>
@@ -2360,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>141</v>
       </c>
@@ -2368,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>142</v>
       </c>
@@ -2376,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>143</v>
       </c>
@@ -2384,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>144</v>
       </c>
@@ -2392,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>145</v>
       </c>
@@ -2400,7 +2413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>146</v>
       </c>
@@ -2408,7 +2421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>147</v>
       </c>
@@ -2416,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>148</v>
       </c>
@@ -2424,7 +2437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -2432,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>150</v>
       </c>
@@ -2440,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>151</v>
       </c>
@@ -2448,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>152</v>
       </c>
@@ -2456,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>153</v>
       </c>
@@ -2464,7 +2477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>154</v>
       </c>
@@ -2472,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -2480,7 +2493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>156</v>
       </c>
@@ -2488,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>157</v>
       </c>
@@ -2496,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>158</v>
       </c>
@@ -2504,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>159</v>
       </c>
@@ -2512,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>160</v>
       </c>
@@ -2520,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>161</v>
       </c>
@@ -2528,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>162</v>
       </c>
@@ -2536,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>163</v>
       </c>
@@ -2544,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>164</v>
       </c>
@@ -2552,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>165</v>
       </c>
@@ -2560,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>166</v>
       </c>
@@ -2568,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>167</v>
       </c>
@@ -2576,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>168</v>
       </c>
@@ -2584,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>169</v>
       </c>
@@ -2592,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>170</v>
       </c>
@@ -2600,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>171</v>
       </c>
@@ -2608,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>172</v>
       </c>
@@ -2616,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>173</v>
       </c>
@@ -2624,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>174</v>
       </c>
@@ -2632,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>175</v>
       </c>
@@ -2640,7 +2653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>176</v>
       </c>
@@ -2648,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>177</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>178</v>
       </c>
@@ -2664,7 +2677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>179</v>
       </c>
@@ -2672,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>180</v>
       </c>
@@ -2680,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>181</v>
       </c>
@@ -2688,7 +2701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>182</v>
       </c>
@@ -2714,9 +2727,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>221</v>
       </c>
@@ -2724,7 +2737,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -2732,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -2740,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -2748,7 +2761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -2756,7 +2769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>226</v>
       </c>
@@ -2764,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>227</v>
       </c>
@@ -2772,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>228</v>
       </c>
@@ -2780,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>229</v>
       </c>
@@ -2801,9 +2814,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>188</v>
       </c>
@@ -2811,7 +2824,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -2819,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -2827,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -2835,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -2851,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -2859,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>195</v>
       </c>
@@ -2867,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>196</v>
       </c>
@@ -2875,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>197</v>
       </c>
@@ -2883,7 +2896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -2891,7 +2904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -2899,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>200</v>
       </c>
@@ -2907,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>201</v>
       </c>
@@ -2915,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>202</v>
       </c>
@@ -2923,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>203</v>
       </c>
@@ -2931,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>204</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>205</v>
       </c>
@@ -2947,7 +2960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>206</v>
       </c>
@@ -2955,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>207</v>
       </c>
@@ -2963,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>208</v>
       </c>
@@ -2971,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>209</v>
       </c>
@@ -2979,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>210</v>
       </c>
@@ -2987,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>211</v>
       </c>
@@ -2995,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>212</v>
       </c>
@@ -3003,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>213</v>
       </c>
@@ -3011,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -3019,7 +3032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>214</v>
       </c>
@@ -3027,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -3035,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>216</v>
       </c>
@@ -3043,7 +3056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -3072,9 +3085,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>219</v>
       </c>
@@ -3082,7 +3095,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3090,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3098,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3127,9 +3140,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -3137,7 +3150,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -3154,13 +3167,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C358E473-EC7A-41C0-8602-044D340269A5}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>261</v>
       </c>
@@ -3168,7 +3181,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -3176,7 +3189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -3184,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>233</v>
       </c>
@@ -3192,7 +3205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -3200,7 +3213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>235</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>236</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -3224,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>238</v>
       </c>
@@ -3232,7 +3245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>239</v>
       </c>
@@ -3240,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -3248,7 +3261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>241</v>
       </c>
@@ -3256,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>242</v>
       </c>
@@ -3264,7 +3277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>243</v>
       </c>
@@ -3272,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>244</v>
       </c>
@@ -3280,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>245</v>
       </c>
@@ -3288,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>246</v>
       </c>
@@ -3296,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>247</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>248</v>
       </c>
@@ -3325,9 +3338,9 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>260</v>
       </c>
@@ -3335,7 +3348,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -3343,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>250</v>
       </c>
@@ -3351,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>251</v>
       </c>
@@ -3359,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>252</v>
       </c>
@@ -3367,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>253</v>
       </c>
@@ -3375,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>254</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>255</v>
       </c>
@@ -3391,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>256</v>
       </c>
@@ -3412,9 +3425,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>259</v>
       </c>
@@ -3423,7 +3436,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3431,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3439,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3447,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3455,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -3463,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2030</v>
       </c>
@@ -3471,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2035</v>
       </c>
@@ -3479,7 +3492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2040</v>
       </c>
@@ -3487,7 +3500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2045</v>
       </c>
@@ -3495,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Fixed small error, where "Res_PV_Utitlity_Tracking" in User Input file was dropped, because "RES" needs to be in capital letters. Also added missing D_PHS_Residual to TagTechnologyToSector
</commit_message>
<xml_diff>
--- a/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
+++ b/GENeSYS-MOD_User_Input_Settings_v04_kh_08-09-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\GENeSYS-MOD new\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{073028ED-85D4-4E35-8EB7-3223E316B965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DF9EB7-484D-4286-85B1-53126D7D394B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -504,9 +504,6 @@
     <t>RES_PV_Utility_Opt</t>
   </si>
   <si>
-    <t>Res_PV_Utility_Tracking</t>
-  </si>
-  <si>
     <t>RES_Residues</t>
   </si>
   <si>
@@ -826,6 +823,9 @@
   </si>
   <si>
     <t>World</t>
+  </si>
+  <si>
+    <t>RES_PV_Utility_Tracking</t>
   </si>
 </sst>
 </file>
@@ -869,16 +869,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -894,7 +893,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1192,18 +1191,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -1211,10 +1210,10 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
@@ -1540,21 +1539,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2486,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>155</v>
+        <v>262</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2495,7 +2494,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2503,7 +2502,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2511,7 +2510,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2519,7 +2518,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2527,7 +2526,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2535,7 +2534,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2543,7 +2542,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2551,7 +2550,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2559,7 +2558,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2567,7 +2566,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -2575,7 +2574,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -2583,7 +2582,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -2591,7 +2590,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -2599,7 +2598,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -2607,7 +2606,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -2615,7 +2614,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -2623,7 +2622,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -2631,7 +2630,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -2639,7 +2638,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -2647,7 +2646,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -2655,7 +2654,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2663,7 +2662,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2671,7 +2670,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2679,7 +2678,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2687,7 +2686,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2695,7 +2694,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2703,7 +2702,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2727,19 +2726,19 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2747,7 +2746,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2755,7 +2754,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2763,7 +2762,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2771,7 +2770,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2779,7 +2778,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2787,7 +2786,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2795,7 +2794,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2814,19 +2813,19 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2834,7 +2833,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2842,7 +2841,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2850,7 +2849,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2858,7 +2857,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2866,7 +2865,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2874,7 +2873,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2882,7 +2881,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2890,7 +2889,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2898,7 +2897,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2906,7 +2905,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2914,7 +2913,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2922,7 +2921,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2930,7 +2929,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2938,7 +2937,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2946,7 +2945,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2954,7 +2953,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2962,7 +2961,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2970,7 +2969,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2978,7 +2977,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2986,7 +2985,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2994,7 +2993,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3002,7 +3001,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3010,7 +3009,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3018,7 +3017,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3026,7 +3025,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3034,7 +3033,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3042,7 +3041,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3050,7 +3049,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3058,7 +3057,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3085,14 +3084,14 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3140,19 +3139,19 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3171,19 +3170,19 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3191,7 +3190,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3199,7 +3198,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3207,7 +3206,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3215,7 +3214,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3223,7 +3222,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3231,7 +3230,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3239,7 +3238,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3247,7 +3246,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3255,7 +3254,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3263,7 +3262,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3271,7 +3270,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3279,7 +3278,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3287,7 +3286,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3295,7 +3294,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3303,7 +3302,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3311,7 +3310,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3319,7 +3318,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3338,19 +3337,19 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3358,7 +3357,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3366,7 +3365,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3374,7 +3373,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3382,7 +3381,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3390,7 +3389,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3398,7 +3397,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3406,7 +3405,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3425,11 +3424,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>

</xml_diff>